<commit_message>
Better cumulation of Kpis
</commit_message>
<xml_diff>
--- a/public/sample_uploads/allocate_account_entries/capital_commitments.xlsx
+++ b/public/sample_uploads/allocate_account_entries/capital_commitments.xlsx
@@ -22,8 +22,7 @@
 <file path=xl/comments1.xml><?xml version="1.0" encoding="utf-8"?>
 <comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing">
   <authors>
-    <author>Author</author>
-    <author>thimm</author>
+    <author>Unknown Author</author>
   </authors>
   <commentList>
     <comment ref="A1" authorId="0">
@@ -95,7 +94,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="D1" authorId="1">
+    <comment ref="D1" authorId="0">
       <text>
         <r>
           <rPr>
@@ -498,7 +497,7 @@
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="79" uniqueCount="45">
   <si>
-    <t xml:space="preserve">Investor *</t>
+    <t xml:space="preserve">Stakeholder *</t>
   </si>
   <si>
     <t xml:space="preserve">Fund *</t>
@@ -785,27 +784,27 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="22" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="22" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="165" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="165" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -813,7 +812,7 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="21" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="21" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -821,7 +820,7 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -842,23 +841,6 @@
     <cellStyle name="Normal 4" xfId="23"/>
     <cellStyle name="*unknown*" xfId="20" builtinId="8"/>
   </cellStyles>
-  <dxfs count="2">
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <bgColor rgb="FF000000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FF0563C1"/>
-          <bgColor rgb="FF000000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-  </dxfs>
   <colors>
     <indexedColors>
       <rgbColor rgb="FF000000"/>
@@ -1102,10 +1084,10 @@
   <dimension ref="A1:U15"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="false" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B6" activeCellId="0" sqref="B6"/>
+      <selection pane="topLeft" activeCell="A2" activeCellId="0" sqref="A2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.00390625" defaultRowHeight="12.75" customHeight="true" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="9.00390625" defaultRowHeight="12.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="8.62"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="24.69"/>

</xml_diff>

<commit_message>
Added get_form_type in the import_utils
</commit_message>
<xml_diff>
--- a/public/sample_uploads/allocate_account_entries/capital_commitments.xlsx
+++ b/public/sample_uploads/allocate_account_entries/capital_commitments.xlsx
@@ -495,7 +495,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="79" uniqueCount="45">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="87" uniqueCount="47">
   <si>
     <t xml:space="preserve">Stakeholder *</t>
   </si>
@@ -560,6 +560,9 @@
     <t xml:space="preserve">Feeder Fund</t>
   </si>
   <si>
+    <t xml:space="preserve">Form Tag</t>
+  </si>
+  <si>
     <t xml:space="preserve">AA TEST</t>
   </si>
   <si>
@@ -582,6 +585,9 @@
   </si>
   <si>
     <t xml:space="preserve">No</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Default</t>
   </si>
   <si>
     <t xml:space="preserve">AB</t>
@@ -1081,10 +1087,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:U15"/>
+  <dimension ref="A1:V15"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="false" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A2" activeCellId="0" sqref="A2"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="false" defaultGridColor="true" view="normal" topLeftCell="M1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="V2" activeCellId="0" sqref="V2:V8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.00390625" defaultRowHeight="12.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -1176,32 +1182,35 @@
       <c r="U1" s="1" t="s">
         <v>20</v>
       </c>
+      <c r="V1" s="1" t="s">
+        <v>21</v>
+      </c>
     </row>
     <row r="2" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="4" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="C2" s="5" t="n">
         <v>50000000</v>
       </c>
       <c r="D2" s="5"/>
       <c r="E2" s="5" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="F2" s="1" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="G2" s="1" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="H2" s="1" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="I2" s="1" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="K2" s="6" t="n">
         <v>45017</v>
@@ -1209,40 +1218,43 @@
       <c r="L2" s="7"/>
       <c r="Q2" s="4"/>
       <c r="R2" s="1" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="S2" s="1" t="n">
         <v>0.142857142857143</v>
       </c>
       <c r="T2" s="1" t="n">
         <v>0.136485151684219</v>
+      </c>
+      <c r="V2" s="1" t="s">
+        <v>30</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="4" t="s">
-        <v>29</v>
+        <v>31</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="C3" s="5" t="n">
         <v>100000000</v>
       </c>
       <c r="D3" s="5"/>
       <c r="E3" s="5" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="F3" s="1" t="s">
-        <v>30</v>
+        <v>32</v>
       </c>
       <c r="G3" s="1" t="s">
-        <v>31</v>
+        <v>33</v>
       </c>
       <c r="H3" s="1" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="I3" s="1" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="K3" s="6" t="n">
         <v>45017</v>
@@ -1250,40 +1262,43 @@
       <c r="L3" s="7"/>
       <c r="Q3" s="4"/>
       <c r="R3" s="1" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="S3" s="1" t="n">
         <v>0.285714285714286</v>
       </c>
       <c r="T3" s="1" t="n">
         <v>0.272970303368438</v>
+      </c>
+      <c r="V3" s="1" t="s">
+        <v>30</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="4" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="C4" s="5" t="n">
         <v>50000000</v>
       </c>
       <c r="D4" s="5"/>
       <c r="E4" s="5" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="F4" s="1" t="s">
-        <v>33</v>
+        <v>35</v>
       </c>
       <c r="G4" s="1" t="s">
-        <v>34</v>
+        <v>36</v>
       </c>
       <c r="H4" s="1" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="I4" s="1" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="K4" s="6" t="n">
         <v>45017</v>
@@ -1291,40 +1306,43 @@
       <c r="L4" s="7"/>
       <c r="Q4" s="4"/>
       <c r="R4" s="1" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="S4" s="1" t="n">
         <v>0.142857142857143</v>
       </c>
       <c r="T4" s="1" t="n">
         <v>0.16207611762501</v>
+      </c>
+      <c r="V4" s="1" t="s">
+        <v>30</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="4" t="s">
-        <v>35</v>
+        <v>37</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="C5" s="5" t="n">
         <v>100000000</v>
       </c>
       <c r="D5" s="5"/>
       <c r="E5" s="5" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="F5" s="1" t="s">
-        <v>36</v>
+        <v>38</v>
       </c>
       <c r="G5" s="1" t="s">
-        <v>37</v>
+        <v>39</v>
       </c>
       <c r="H5" s="1" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="I5" s="1" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="K5" s="6" t="n">
         <v>45017</v>
@@ -1332,40 +1350,43 @@
       <c r="L5" s="7"/>
       <c r="Q5" s="8"/>
       <c r="R5" s="1" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="S5" s="1" t="n">
         <v>0.285714285714286</v>
       </c>
       <c r="T5" s="1" t="n">
         <v>0.272970303368438</v>
+      </c>
+      <c r="V5" s="1" t="s">
+        <v>30</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="4" t="s">
-        <v>38</v>
+        <v>40</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="C6" s="5" t="n">
         <v>50000000</v>
       </c>
       <c r="D6" s="5"/>
       <c r="E6" s="5" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="F6" s="1" t="s">
-        <v>39</v>
+        <v>41</v>
       </c>
       <c r="G6" s="1" t="s">
-        <v>40</v>
+        <v>42</v>
       </c>
       <c r="H6" s="1" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="I6" s="1" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="K6" s="6" t="n">
         <v>45017</v>
@@ -1373,40 +1394,43 @@
       <c r="L6" s="7"/>
       <c r="Q6" s="8"/>
       <c r="R6" s="1" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="S6" s="1" t="n">
         <v>0.142857142857143</v>
       </c>
       <c r="T6" s="1" t="n">
         <v>0.155498123953896</v>
+      </c>
+      <c r="V6" s="1" t="s">
+        <v>30</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="1" t="s">
-        <v>35</v>
+        <v>37</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>41</v>
+        <v>43</v>
       </c>
       <c r="C7" s="5" t="n">
         <v>1000000</v>
       </c>
       <c r="D7" s="9"/>
       <c r="E7" s="5" t="s">
-        <v>42</v>
+        <v>44</v>
       </c>
       <c r="F7" s="1" t="s">
-        <v>43</v>
+        <v>45</v>
       </c>
       <c r="G7" s="1" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="H7" s="1" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="I7" s="1" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="K7" s="6" t="n">
         <v>45017</v>
@@ -1414,37 +1438,40 @@
       <c r="L7" s="7"/>
       <c r="Q7" s="8"/>
       <c r="R7" s="1" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="U7" s="1" t="s">
-        <v>22</v>
+        <v>23</v>
+      </c>
+      <c r="V7" s="1" t="s">
+        <v>30</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="1" t="s">
-        <v>35</v>
+        <v>37</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>41</v>
+        <v>43</v>
       </c>
       <c r="C8" s="5" t="n">
         <v>625000</v>
       </c>
       <c r="D8" s="9"/>
       <c r="E8" s="5" t="s">
-        <v>42</v>
+        <v>44</v>
       </c>
       <c r="F8" s="1" t="s">
-        <v>44</v>
+        <v>46</v>
       </c>
       <c r="G8" s="1" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="H8" s="1" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="I8" s="1" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="K8" s="6" t="n">
         <v>45017</v>
@@ -1452,10 +1479,13 @@
       <c r="L8" s="7"/>
       <c r="Q8" s="8"/>
       <c r="R8" s="1" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="U8" s="1" t="s">
-        <v>22</v>
+        <v>23</v>
+      </c>
+      <c r="V8" s="1" t="s">
+        <v>30</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="13.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">

</xml_diff>